<commit_message>
fix: fix ssh bras on windows
</commit_message>
<xml_diff>
--- a/du_lieu.xlsx
+++ b/du_lieu.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4579,6 +4579,87 @@
         </is>
       </c>
     </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>L T</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> daihostvlg</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2024-05-07 18:18:52</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tài khoản đã mở cước - Không thể thực hiện mở cước</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Group: Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>L T</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> daihostvlg </t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2024-05-07 19:47:57</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tài khoản đã mở cước - Không thể thực hiện mở cước</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Chat trực tiếp với Bot</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>L T</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> daihostvlg</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2024-05-07 20:49:40</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tài khoản đã mở cước - Không thể thực hiện mở cước</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Group: Test</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>